<commit_message>
[Update] Test Case Reset
</commit_message>
<xml_diff>
--- a/docs/[TC] Reset.xlsx
+++ b/docs/[TC] Reset.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B49C6C-805F-455E-A89B-455C5300A320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Test Case no.</t>
   </si>
@@ -45,20 +46,17 @@
     <t>expectedParkingTime, coinValue</t>
   </si>
   <si>
-    <t>Should display 0 min when the BUY button is pressed</t>
-  </si>
-  <si>
     <t>Display is cleared after cancellation</t>
   </si>
   <si>
-    <t>Should display 0 min when the CANCEL button is pressed</t>
+    <t>expectedParkingTime = 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,46 +193,46 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -244,6 +242,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -290,7 +296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,9 +328,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,6 +380,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -531,34 +573,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="48.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="47.25">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="13"/>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
@@ -566,83 +609,83 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="5">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" ht="47.25">
-      <c r="A3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75">
-      <c r="A4" s="11">
-        <v>2</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" ht="47.25">
-      <c r="A5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="E2:F3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:D5"/>
     <mergeCell ref="E4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="E2:F3"/>
     <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -651,24 +694,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>